<commit_message>
Updated BOM with debounced switch parts
</commit_message>
<xml_diff>
--- a/meng-spad-quenching/aqc-dac-io-board-rev1-bom.xlsx
+++ b/meng-spad-quenching/aqc-dac-io-board-rev1-bom.xlsx
@@ -15,7 +15,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="aqc_dac_io_board_rev1_bom" localSheetId="0">Sheet1!$A$1:$G$22</definedName>
+    <definedName name="aqc_dac_io_board_rev1_bom" localSheetId="0">Sheet1!$A$1:$G$25</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="124">
   <si>
     <t>Part</t>
   </si>
@@ -131,15 +131,9 @@
     <t>DNP</t>
   </si>
   <si>
-    <t>R10</t>
-  </si>
-  <si>
     <t>2k2</t>
   </si>
   <si>
-    <t>R11</t>
-  </si>
-  <si>
     <t>STM32</t>
   </si>
   <si>
@@ -179,9 +173,6 @@
     <t>Cost/Qty.</t>
   </si>
   <si>
-    <t>C1, C2, C3, C5, C6, C8, C10</t>
-  </si>
-  <si>
     <t>C7, C9, C11</t>
   </si>
   <si>
@@ -212,9 +203,6 @@
     <t>aqc-dac-io-board-rev1 BOM</t>
   </si>
   <si>
-    <t>16V</t>
-  </si>
-  <si>
     <t>1/8W</t>
   </si>
   <si>
@@ -236,9 +224,6 @@
     <t>Generic</t>
   </si>
   <si>
-    <t>1/8W, 1%</t>
-  </si>
-  <si>
     <t>LT1366CS8#PBF-ND</t>
   </si>
   <si>
@@ -261,6 +246,177 @@
   </si>
   <si>
     <t>Comment</t>
+  </si>
+  <si>
+    <t>Generic/Already Have</t>
+  </si>
+  <si>
+    <t>R12</t>
+  </si>
+  <si>
+    <t>R13</t>
+  </si>
+  <si>
+    <t>4k7</t>
+  </si>
+  <si>
+    <t>100k</t>
+  </si>
+  <si>
+    <t>C1, C2, C3, C5, C6, C8, C10, C12, C13</t>
+  </si>
+  <si>
+    <t>S1</t>
+  </si>
+  <si>
+    <t>TAC SW TH</t>
+  </si>
+  <si>
+    <t>IC4</t>
+  </si>
+  <si>
+    <t>74AHC1G14</t>
+  </si>
+  <si>
+    <t>SOT23-5</t>
+  </si>
+  <si>
+    <t>296-35922-1-ND</t>
+  </si>
+  <si>
+    <t>IC SNGL SCHM-TRG INV GATESOT23-5</t>
+  </si>
+  <si>
+    <t>36-5000-ND</t>
+  </si>
+  <si>
+    <t>TEST POINT PC MINI .040"D RED</t>
+  </si>
+  <si>
+    <t>TH</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>TEST POINT PC MINI .040"D BLACK</t>
+  </si>
+  <si>
+    <t>36-5001-ND</t>
+  </si>
+  <si>
+    <t>36-5117-ND</t>
+  </si>
+  <si>
+    <t>TEST POINT PC MINIATURE T/H BLUE</t>
+  </si>
+  <si>
+    <t>MCP4725A0T-E/CHCT-ND</t>
+  </si>
+  <si>
+    <t>12 Bit Digital to Analog Converter</t>
+  </si>
+  <si>
+    <t>587-4917-1-ND</t>
+  </si>
+  <si>
+    <t>CAP CER 4.7UF 10V X7R 0805</t>
+  </si>
+  <si>
+    <t>311-5.11KHRCT-ND</t>
+  </si>
+  <si>
+    <t>RES SMD 5.11K OHM 1% 1/10W 0603</t>
+  </si>
+  <si>
+    <t>311-15.0KHRCT-ND</t>
+  </si>
+  <si>
+    <t>RES SMD 15K OHM 1% 1/10W 0603</t>
+  </si>
+  <si>
+    <t>311-10.0KHRCT-ND</t>
+  </si>
+  <si>
+    <t>RES SMD 10K OHM 1% 1/10W 0603</t>
+  </si>
+  <si>
+    <t>RNCP0603FTD100RCT-ND</t>
+  </si>
+  <si>
+    <t>RES SMD 100 OHM 1% 1/8W 0603</t>
+  </si>
+  <si>
+    <t>311-2.20KHRCT-ND</t>
+  </si>
+  <si>
+    <t>RES SMD 2.2K OHM 1% 1/10W 0603</t>
+  </si>
+  <si>
+    <t>R10, R11</t>
+  </si>
+  <si>
+    <t>311-0.0GRCT-ND</t>
+  </si>
+  <si>
+    <t>RES SMD 0.0OHM JUMPER 1/10W 0603</t>
+  </si>
+  <si>
+    <t>311-4.70KHRCT-ND</t>
+  </si>
+  <si>
+    <t>RES SMD 4.7K OHM 1% 1/10W 0603</t>
+  </si>
+  <si>
+    <t>311-100KHRCT-ND</t>
+  </si>
+  <si>
+    <t>RES SMD 100K OHM 1% 1/10W 0603</t>
+  </si>
+  <si>
+    <t>1/10W</t>
+  </si>
+  <si>
+    <t>1/10W, 1%</t>
+  </si>
+  <si>
+    <t>450-1804-ND</t>
+  </si>
+  <si>
+    <t>SWITCH TACTILE SPST-NO 0.05A 24V</t>
+  </si>
+  <si>
+    <t>1212-1103-ND</t>
+  </si>
+  <si>
+    <t>SOCKET 4.2 MM SOLDER TAIL SINGLE</t>
+  </si>
+  <si>
+    <t>WM5534-ND</t>
+  </si>
+  <si>
+    <t>CONN SMA JACK 50 OHM EDGE MNT</t>
+  </si>
+  <si>
+    <t>10V</t>
+  </si>
+  <si>
+    <t>497-15981-ND</t>
+  </si>
+  <si>
+    <t>BOARD NUCLEO STM32F303K8T6</t>
+  </si>
+  <si>
+    <t>CAP CER 0.1UF 25V X7R 0603</t>
+  </si>
+  <si>
+    <t>490-1524-1-ND</t>
+  </si>
+  <si>
+    <t>CAP CER 10000PF 25V X7R 0603</t>
+  </si>
+  <si>
+    <t>1276-1132-1-ND</t>
   </si>
 </sst>
 </file>
@@ -270,7 +426,7 @@
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -293,8 +449,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -306,8 +470,13 @@
         <fgColor rgb="FFFFFFCC"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -330,21 +499,39 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="2" applyFont="1"/>
     <xf numFmtId="44" fontId="0" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="3" fillId="3" borderId="2" xfId="3" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
+    <cellStyle name="Calculation" xfId="3" builtinId="22"/>
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Note" xfId="2" builtinId="10"/>
@@ -629,40 +816,40 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K26"/>
+  <dimension ref="A1:K29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="59" customWidth="1"/>
-    <col min="3" max="3" width="26.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.140625" customWidth="1"/>
+    <col min="4" max="4" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="29.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="35.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11" style="3" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="4.7109375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="10.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B2" s="3" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>0</v>
@@ -671,28 +858,28 @@
         <v>1</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="F3" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H3" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="I3" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="J3" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="I3" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>43</v>
-      </c>
       <c r="K3" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -700,29 +887,35 @@
         <v>1</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>44</v>
+        <v>72</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>3</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>55</v>
+        <v>117</v>
       </c>
       <c r="E4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="5"/>
+      <c r="F4" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="H4" s="5">
+        <v>0.09</v>
+      </c>
       <c r="I4" s="4">
-        <v>7</v>
-      </c>
-      <c r="J4" s="5">
+        <v>9</v>
+      </c>
+      <c r="J4" s="6">
         <f>H4*I4</f>
-        <v>0</v>
+        <v>0.80999999999999994</v>
       </c>
       <c r="K4" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -737,48 +930,66 @@
         <v>6</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>55</v>
+        <v>117</v>
       </c>
       <c r="E5" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="5"/>
+      <c r="F5" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="H5" s="5">
+        <v>0.09</v>
+      </c>
       <c r="I5" s="4">
         <v>1</v>
       </c>
-      <c r="J5" s="5">
+      <c r="J5" s="6">
         <f>H5*I5</f>
-        <v>0</v>
+        <v>0.09</v>
       </c>
       <c r="K5" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6">
-        <f t="shared" ref="A6:A24" si="0">A5+1</f>
+        <f t="shared" ref="A6:A27" si="0">A5+1</f>
         <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C6" t="s">
         <v>7</v>
       </c>
       <c r="D6" t="s">
-        <v>55</v>
+        <v>117</v>
       </c>
       <c r="E6" t="s">
         <v>8</v>
       </c>
+      <c r="F6" t="s">
+        <v>91</v>
+      </c>
+      <c r="G6" t="s">
+        <v>90</v>
+      </c>
+      <c r="H6" s="3">
+        <v>0.22</v>
+      </c>
       <c r="I6">
         <v>3</v>
       </c>
-      <c r="J6" s="3">
+      <c r="J6" s="6">
         <f>H6*I6</f>
-        <v>0</v>
+        <v>0.66</v>
+      </c>
+      <c r="K6" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -792,14 +1003,17 @@
       <c r="C7" t="s">
         <v>10</v>
       </c>
+      <c r="D7" t="s">
+        <v>83</v>
+      </c>
       <c r="E7" t="s">
         <v>11</v>
       </c>
       <c r="F7" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="G7" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="H7" s="3">
         <v>7.34</v>
@@ -807,8 +1021,8 @@
       <c r="I7">
         <v>1</v>
       </c>
-      <c r="J7" s="3">
-        <f t="shared" ref="J7:J13" si="1">H7*I7</f>
+      <c r="J7" s="6">
+        <f t="shared" ref="J7:J25" si="1">H7*I7</f>
         <v>7.34</v>
       </c>
     </row>
@@ -823,14 +1037,17 @@
       <c r="C8" t="s">
         <v>13</v>
       </c>
+      <c r="D8" t="s">
+        <v>83</v>
+      </c>
       <c r="E8" t="s">
         <v>14</v>
       </c>
       <c r="F8" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="G8" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="H8" s="3">
         <v>0.43</v>
@@ -838,7 +1055,7 @@
       <c r="I8">
         <v>1</v>
       </c>
-      <c r="J8" s="3">
+      <c r="J8" s="6">
         <f t="shared" si="1"/>
         <v>0.43</v>
       </c>
@@ -854,14 +1071,17 @@
       <c r="C9" t="s">
         <v>16</v>
       </c>
+      <c r="D9" t="s">
+        <v>83</v>
+      </c>
       <c r="E9" t="s">
         <v>17</v>
       </c>
       <c r="F9" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="G9" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="H9" s="3">
         <v>5.13</v>
@@ -869,7 +1089,7 @@
       <c r="I9">
         <v>1</v>
       </c>
-      <c r="J9" s="3">
+      <c r="J9" s="6">
         <f t="shared" si="1"/>
         <v>5.13</v>
       </c>
@@ -880,362 +1100,640 @@
         <v>7</v>
       </c>
       <c r="B10" t="s">
-        <v>46</v>
+        <v>75</v>
       </c>
       <c r="C10" t="s">
+        <v>76</v>
+      </c>
+      <c r="D10" t="s">
+        <v>83</v>
+      </c>
+      <c r="E10" t="s">
+        <v>77</v>
+      </c>
+      <c r="F10" t="s">
+        <v>79</v>
+      </c>
+      <c r="G10" t="s">
+        <v>78</v>
+      </c>
+      <c r="H10" s="3">
+        <v>0.36</v>
+      </c>
+      <c r="I10">
+        <v>1</v>
+      </c>
+      <c r="J10" s="6">
+        <f t="shared" si="1"/>
+        <v>0.36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="B11" t="s">
+        <v>43</v>
+      </c>
+      <c r="C11" t="s">
         <v>18</v>
       </c>
-      <c r="D10" t="s">
-        <v>56</v>
-      </c>
-      <c r="E10" t="s">
+      <c r="D11" t="s">
+        <v>52</v>
+      </c>
+      <c r="E11" t="s">
         <v>19</v>
       </c>
-      <c r="I10">
+      <c r="F11" t="s">
+        <v>99</v>
+      </c>
+      <c r="G11" t="s">
+        <v>98</v>
+      </c>
+      <c r="H11" s="3">
+        <v>0.09</v>
+      </c>
+      <c r="I11">
         <v>2</v>
       </c>
-      <c r="J10" s="3">
+      <c r="J11" s="6">
+        <f t="shared" si="1"/>
+        <v>0.18</v>
+      </c>
+      <c r="K11" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="B12" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" t="s">
+        <v>21</v>
+      </c>
+      <c r="D12" t="s">
+        <v>110</v>
+      </c>
+      <c r="E12" t="s">
+        <v>19</v>
+      </c>
+      <c r="F12" t="s">
+        <v>95</v>
+      </c>
+      <c r="G12" t="s">
+        <v>94</v>
+      </c>
+      <c r="H12" s="3">
+        <v>0.09</v>
+      </c>
+      <c r="I12">
+        <v>1</v>
+      </c>
+      <c r="J12" s="6">
+        <f t="shared" si="1"/>
+        <v>0.09</v>
+      </c>
+      <c r="K12" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="B13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" t="s">
+        <v>23</v>
+      </c>
+      <c r="D13" t="s">
+        <v>110</v>
+      </c>
+      <c r="E13" t="s">
+        <v>19</v>
+      </c>
+      <c r="F13" t="s">
+        <v>93</v>
+      </c>
+      <c r="G13" t="s">
+        <v>92</v>
+      </c>
+      <c r="H13" s="3">
+        <v>0.09</v>
+      </c>
+      <c r="I13">
+        <v>1</v>
+      </c>
+      <c r="J13" s="6">
+        <f t="shared" si="1"/>
+        <v>0.09</v>
+      </c>
+      <c r="K13" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="B14" t="s">
+        <v>49</v>
+      </c>
+      <c r="C14" t="s">
+        <v>24</v>
+      </c>
+      <c r="D14" t="s">
+        <v>110</v>
+      </c>
+      <c r="E14" t="s">
+        <v>19</v>
+      </c>
+      <c r="F14" t="s">
+        <v>97</v>
+      </c>
+      <c r="G14" t="s">
+        <v>96</v>
+      </c>
+      <c r="H14" s="3">
+        <v>0.09</v>
+      </c>
+      <c r="I14">
+        <v>2</v>
+      </c>
+      <c r="J14" s="6">
+        <f t="shared" si="1"/>
+        <v>0.18</v>
+      </c>
+      <c r="K14" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="H15" s="5">
+        <v>0.09</v>
+      </c>
+      <c r="I15" s="4">
+        <v>2</v>
+      </c>
+      <c r="J15" s="6">
+        <f t="shared" si="1"/>
+        <v>0.18</v>
+      </c>
+      <c r="K15" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="H16" s="5">
+        <v>0</v>
+      </c>
+      <c r="I16" s="4">
+        <v>1</v>
+      </c>
+      <c r="J16" s="6">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="B11" t="s">
-        <v>20</v>
-      </c>
-      <c r="C11" t="s">
-        <v>21</v>
-      </c>
-      <c r="D11" t="s">
-        <v>63</v>
-      </c>
-      <c r="E11" t="s">
-        <v>19</v>
-      </c>
-      <c r="I11">
-        <v>1</v>
-      </c>
-      <c r="J11" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="B12" t="s">
-        <v>22</v>
-      </c>
-      <c r="C12" t="s">
-        <v>23</v>
-      </c>
-      <c r="D12" t="s">
-        <v>63</v>
-      </c>
-      <c r="E12" t="s">
-        <v>19</v>
-      </c>
-      <c r="I12">
-        <v>1</v>
-      </c>
-      <c r="J12" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="B13" t="s">
-        <v>52</v>
-      </c>
-      <c r="C13" t="s">
-        <v>24</v>
-      </c>
-      <c r="D13" t="s">
-        <v>63</v>
-      </c>
-      <c r="E13" t="s">
-        <v>19</v>
-      </c>
-      <c r="I13">
-        <v>2</v>
-      </c>
-      <c r="J13" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="4">
-        <f t="shared" si="0"/>
-        <v>11</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
-      <c r="H14" s="5"/>
-      <c r="I14" s="4">
-        <v>2</v>
-      </c>
-      <c r="J14" s="5">
-        <f>H14*I14</f>
-        <v>0</v>
-      </c>
-      <c r="K14" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="4">
-        <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="F15" s="4"/>
-      <c r="G15" s="4"/>
-      <c r="H15" s="5"/>
-      <c r="I15" s="4">
-        <v>1</v>
-      </c>
-      <c r="J15" s="5">
-        <f>H15*I15</f>
-        <v>0</v>
-      </c>
-      <c r="K15" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <f t="shared" si="0"/>
-        <v>13</v>
-      </c>
-      <c r="B16" t="s">
+      <c r="K16" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="B17" t="s">
+        <v>102</v>
+      </c>
+      <c r="C17" t="s">
         <v>28</v>
       </c>
-      <c r="C16" t="s">
-        <v>29</v>
-      </c>
-      <c r="D16" t="s">
-        <v>56</v>
-      </c>
-      <c r="E16" t="s">
-        <v>19</v>
-      </c>
-      <c r="I16">
-        <v>1</v>
-      </c>
-      <c r="J16" s="3">
-        <f>H16*I16</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <f t="shared" si="0"/>
-        <v>14</v>
-      </c>
-      <c r="B17" t="s">
-        <v>30</v>
-      </c>
-      <c r="C17" t="s">
-        <v>29</v>
-      </c>
       <c r="D17" t="s">
-        <v>56</v>
+        <v>109</v>
       </c>
       <c r="E17" t="s">
         <v>19</v>
       </c>
+      <c r="F17" t="s">
+        <v>101</v>
+      </c>
+      <c r="G17" t="s">
+        <v>100</v>
+      </c>
+      <c r="H17" s="3">
+        <v>0.09</v>
+      </c>
       <c r="I17">
-        <v>1</v>
-      </c>
-      <c r="J17" s="3">
-        <f>H17*I17</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="J17" s="6">
+        <f t="shared" si="1"/>
+        <v>0.18</v>
+      </c>
+      <c r="K17" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
       <c r="B18" t="s">
-        <v>33</v>
+        <v>68</v>
       </c>
       <c r="C18" t="s">
-        <v>57</v>
+        <v>70</v>
+      </c>
+      <c r="D18" t="s">
+        <v>109</v>
+      </c>
+      <c r="E18" t="s">
+        <v>19</v>
+      </c>
+      <c r="F18" t="s">
+        <v>106</v>
+      </c>
+      <c r="G18" t="s">
+        <v>105</v>
+      </c>
+      <c r="H18" s="3">
+        <v>0.09</v>
       </c>
       <c r="I18">
         <v>1</v>
       </c>
-      <c r="J18" s="3">
-        <f>H18*I18</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J18" s="6">
+        <f t="shared" si="1"/>
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
       <c r="B19" t="s">
-        <v>34</v>
+        <v>69</v>
       </c>
       <c r="C19" t="s">
-        <v>58</v>
+        <v>71</v>
+      </c>
+      <c r="D19" t="s">
+        <v>109</v>
+      </c>
+      <c r="E19" t="s">
+        <v>19</v>
+      </c>
+      <c r="F19" t="s">
+        <v>108</v>
+      </c>
+      <c r="G19" t="s">
+        <v>107</v>
+      </c>
+      <c r="H19" s="3">
+        <v>0.09</v>
       </c>
       <c r="I19">
         <v>1</v>
       </c>
-      <c r="J19" s="3">
-        <f>H19*I19</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J19" s="6">
+        <f t="shared" si="1"/>
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
       <c r="B20" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C20" t="s">
-        <v>59</v>
+        <v>53</v>
+      </c>
+      <c r="D20" t="s">
+        <v>83</v>
+      </c>
+      <c r="E20" t="s">
+        <v>82</v>
+      </c>
+      <c r="F20" t="s">
+        <v>81</v>
+      </c>
+      <c r="G20" t="s">
+        <v>80</v>
+      </c>
+      <c r="H20" s="3">
+        <v>0.32</v>
       </c>
       <c r="I20">
         <v>1</v>
       </c>
-      <c r="J20" s="3">
-        <f>H20*I20</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J20" s="6">
+        <f t="shared" si="1"/>
+        <v>0.32</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
       <c r="B21" t="s">
-        <v>48</v>
+        <v>32</v>
       </c>
       <c r="C21" t="s">
+        <v>54</v>
+      </c>
+      <c r="D21" t="s">
+        <v>83</v>
+      </c>
+      <c r="E21" t="s">
+        <v>82</v>
+      </c>
+      <c r="F21" t="s">
+        <v>84</v>
+      </c>
+      <c r="G21" t="s">
+        <v>85</v>
+      </c>
+      <c r="H21" s="3">
+        <v>0.32</v>
+      </c>
+      <c r="I21">
+        <v>1</v>
+      </c>
+      <c r="J21" s="6">
+        <f t="shared" si="1"/>
+        <v>0.32</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="B22" t="s">
+        <v>33</v>
+      </c>
+      <c r="C22" t="s">
+        <v>55</v>
+      </c>
+      <c r="D22" t="s">
+        <v>83</v>
+      </c>
+      <c r="E22" t="s">
+        <v>82</v>
+      </c>
+      <c r="F22" t="s">
+        <v>87</v>
+      </c>
+      <c r="G22" t="s">
+        <v>86</v>
+      </c>
+      <c r="H22" s="3">
+        <v>0.32</v>
+      </c>
+      <c r="I22">
+        <v>1</v>
+      </c>
+      <c r="J22" s="6">
+        <f t="shared" si="1"/>
+        <v>0.32</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="B23" t="s">
+        <v>45</v>
+      </c>
+      <c r="C23" t="s">
+        <v>44</v>
+      </c>
+      <c r="D23" t="s">
+        <v>83</v>
+      </c>
+      <c r="E23" t="s">
+        <v>34</v>
+      </c>
+      <c r="F23" t="s">
+        <v>89</v>
+      </c>
+      <c r="G23" t="s">
+        <v>88</v>
+      </c>
+      <c r="H23" s="3">
+        <v>0.99</v>
+      </c>
+      <c r="I23">
+        <v>3</v>
+      </c>
+      <c r="J23" s="6">
+        <f t="shared" si="1"/>
+        <v>2.9699999999999998</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="B24" t="s">
+        <v>73</v>
+      </c>
+      <c r="C24" t="s">
+        <v>74</v>
+      </c>
+      <c r="D24" t="s">
+        <v>83</v>
+      </c>
+      <c r="E24" t="s">
+        <v>82</v>
+      </c>
+      <c r="F24" t="s">
+        <v>112</v>
+      </c>
+      <c r="G24" t="s">
+        <v>111</v>
+      </c>
+      <c r="H24" s="3">
+        <v>0.09</v>
+      </c>
+      <c r="I24">
+        <v>1</v>
+      </c>
+      <c r="J24" s="6">
+        <f t="shared" si="1"/>
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="B25" t="s">
+        <v>46</v>
+      </c>
+      <c r="C25" t="s">
         <v>47</v>
       </c>
-      <c r="E21" t="s">
-        <v>36</v>
-      </c>
-      <c r="I21">
-        <v>3</v>
-      </c>
-      <c r="J21" s="3">
-        <f>H21*I21</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <f t="shared" si="0"/>
-        <v>19</v>
-      </c>
-      <c r="B22" t="s">
-        <v>49</v>
-      </c>
-      <c r="C22" t="s">
-        <v>50</v>
-      </c>
-      <c r="E22" t="s">
-        <v>50</v>
-      </c>
-      <c r="I22">
+      <c r="D25" t="s">
+        <v>83</v>
+      </c>
+      <c r="E25" t="s">
+        <v>47</v>
+      </c>
+      <c r="F25" t="s">
+        <v>116</v>
+      </c>
+      <c r="G25" t="s">
+        <v>115</v>
+      </c>
+      <c r="H25" s="3">
+        <v>2.84</v>
+      </c>
+      <c r="I25">
         <v>5</v>
       </c>
-      <c r="J22" s="3">
-        <f>H22*I22</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="B23" t="s">
-        <v>31</v>
-      </c>
-      <c r="C23" t="s">
-        <v>60</v>
-      </c>
-      <c r="E23" t="s">
-        <v>32</v>
-      </c>
-      <c r="I23">
+      <c r="J25" s="6">
+        <f t="shared" si="1"/>
+        <v>14.2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="B26" t="s">
+        <v>29</v>
+      </c>
+      <c r="C26" t="s">
+        <v>56</v>
+      </c>
+      <c r="D26" t="s">
+        <v>83</v>
+      </c>
+      <c r="E26" t="s">
+        <v>30</v>
+      </c>
+      <c r="F26" t="s">
+        <v>119</v>
+      </c>
+      <c r="G26" t="s">
+        <v>118</v>
+      </c>
+      <c r="H26" s="3">
+        <v>9.75</v>
+      </c>
+      <c r="I26">
         <v>1</v>
       </c>
-      <c r="J23" s="3">
-        <f>H23*I23</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <f t="shared" si="0"/>
-        <v>21</v>
-      </c>
-      <c r="B24" t="s">
-        <v>31</v>
-      </c>
-      <c r="C24" t="s">
-        <v>61</v>
-      </c>
-      <c r="E24" t="s">
-        <v>32</v>
-      </c>
-      <c r="I24">
+      <c r="J26" s="6">
+        <f t="shared" ref="J26:J27" si="2">H26*I26</f>
+        <v>9.75</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="B27" t="s">
+        <v>29</v>
+      </c>
+      <c r="C27" t="s">
+        <v>57</v>
+      </c>
+      <c r="D27" t="s">
+        <v>83</v>
+      </c>
+      <c r="E27" t="s">
+        <v>30</v>
+      </c>
+      <c r="F27" t="s">
+        <v>114</v>
+      </c>
+      <c r="G27" t="s">
+        <v>113</v>
+      </c>
+      <c r="H27" s="3">
+        <v>0.81</v>
+      </c>
+      <c r="I27">
         <v>2</v>
       </c>
-      <c r="J24" s="3">
-        <f>H24*I24</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="H26" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="J26" s="3">
-        <f>SUM(J4:J24)</f>
-        <v>12.899999999999999</v>
+      <c r="J27" s="6">
+        <f t="shared" si="2"/>
+        <v>1.62</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="H29" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="J29" s="6">
+        <f>SUM(J4:J27)</f>
+        <v>45.489999999999995</v>
       </c>
     </row>
   </sheetData>

</xml_diff>